<commit_message>
Added report and modified test excels
</commit_message>
<xml_diff>
--- a/Measurements/Test 1 - No obstacles/Statistics2.xlsx
+++ b/Measurements/Test 1 - No obstacles/Statistics2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\CodeFromGithub\SerialPortRead\Vamia-SerialPortReading\Measurements\Test 1 - No obstacles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\code\SerialReading\Measurements\Test 1 - No obstacles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BE941E-3170-4885-AF92-E253642A6EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5ABA5A-31AD-4E48-B0BE-D38AF5100F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,32 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +77,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,17 +118,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1315,6 +1347,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>ESP32 - No obstacles RSSI</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1353,6 +1410,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Real RSSI</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1519,6 +1579,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Computed RSSI</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1759,6 +1822,7 @@
         <c:axId val="1224216672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4157,16 +4221,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:rowOff>100965</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4194,15 +4258,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>49530</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4229,15 +4293,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>112395</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4551,15 +4615,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4574,7 +4642,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4589,7 +4657,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -4613,8 +4681,19 @@
         <f>POWER(10, (B3-$F$1)/(10*$G$1))</f>
         <v>0.26245062966121019</v>
       </c>
+      <c r="I3" s="1">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2">
+        <f>H3*100</f>
+        <v>26.245062966121019</v>
+      </c>
+      <c r="K3" s="3">
+        <f>(J3-I3)/I3</f>
+        <v>0.31225314830605094</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>40</v>
       </c>
@@ -4638,8 +4717,19 @@
         <f t="shared" ref="H4:H21" si="1">POWER(10, (B4-$F$1)/(10*$G$1))</f>
         <v>0.44424141892319974</v>
       </c>
+      <c r="I4" s="1">
+        <v>40</v>
+      </c>
+      <c r="J4" s="2">
+        <f>H4*100</f>
+        <v>44.424141892319973</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K21" si="2">(J4-I4)/I4</f>
+        <v>0.11060354730799933</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -4663,8 +4753,19 @@
         <f t="shared" si="1"/>
         <v>0.78566624593889489</v>
       </c>
+      <c r="I5" s="1">
+        <v>60</v>
+      </c>
+      <c r="J5" s="2">
+        <f>H5*100</f>
+        <v>78.566624593889486</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.30944374323149143</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>80</v>
       </c>
@@ -4688,8 +4789,19 @@
         <f t="shared" si="1"/>
         <v>1.3298710250629042</v>
       </c>
+      <c r="I6" s="1">
+        <v>80</v>
+      </c>
+      <c r="J6" s="2">
+        <f>H6*100</f>
+        <v>132.98710250629043</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66233878132863033</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100</v>
       </c>
@@ -4713,8 +4825,19 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="I7" s="1">
+        <v>100</v>
+      </c>
+      <c r="J7" s="2">
+        <f>H7*100</f>
+        <v>100</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>120</v>
       </c>
@@ -4738,8 +4861,19 @@
         <f t="shared" si="1"/>
         <v>1.0221715980421691</v>
       </c>
+      <c r="I8" s="1">
+        <v>120</v>
+      </c>
+      <c r="J8" s="2">
+        <f>H8*100</f>
+        <v>102.21715980421691</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.14819033496485912</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>140</v>
       </c>
@@ -4763,8 +4897,19 @@
         <f t="shared" si="1"/>
         <v>1.9735043828689784</v>
       </c>
+      <c r="I9" s="1">
+        <v>140</v>
+      </c>
+      <c r="J9" s="2">
+        <f>H9*100</f>
+        <v>197.35043828689786</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4096459877635561</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>160</v>
       </c>
@@ -4788,8 +4933,19 @@
         <f t="shared" si="1"/>
         <v>1.7685569433018593</v>
       </c>
+      <c r="I10" s="1">
+        <v>160</v>
+      </c>
+      <c r="J10" s="2">
+        <f>H10*100</f>
+        <v>176.85569433018594</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.10534808956366212</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>180</v>
       </c>
@@ -4813,8 +4969,19 @@
         <f t="shared" si="1"/>
         <v>2.0619860095022222</v>
       </c>
+      <c r="I11" s="1">
+        <v>180</v>
+      </c>
+      <c r="J11" s="2">
+        <f>H11*100</f>
+        <v>206.19860095022221</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.14554778305679009</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>200</v>
       </c>
@@ -4838,8 +5005,19 @@
         <f t="shared" si="1"/>
         <v>1.8888195803730405</v>
       </c>
+      <c r="I12" s="1">
+        <v>200</v>
+      </c>
+      <c r="J12" s="2">
+        <f>H12*100</f>
+        <v>188.88195803730406</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="2"/>
+        <v>-5.5590209813479702E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>240</v>
       </c>
@@ -4863,8 +5041,19 @@
         <f t="shared" si="1"/>
         <v>1.6200328072641321</v>
       </c>
+      <c r="I13" s="1">
+        <v>240</v>
+      </c>
+      <c r="J13" s="2">
+        <f>H13*100</f>
+        <v>162.00328072641321</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.32498633030661161</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>280</v>
       </c>
@@ -4888,8 +5077,19 @@
         <f t="shared" si="1"/>
         <v>3.5676394072005944</v>
       </c>
+      <c r="I14" s="1">
+        <v>280</v>
+      </c>
+      <c r="J14" s="2">
+        <f>H14*100</f>
+        <v>356.76394072005945</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.27415693114306949</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>320</v>
       </c>
@@ -4913,8 +5113,19 @@
         <f t="shared" si="1"/>
         <v>2.9935772947204904</v>
       </c>
+      <c r="I15" s="1">
+        <v>320</v>
+      </c>
+      <c r="J15" s="2">
+        <f>H15*100</f>
+        <v>299.35772947204902</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.4507095399846823E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>360</v>
       </c>
@@ -4938,8 +5149,19 @@
         <f t="shared" si="1"/>
         <v>3.4902548789595831</v>
       </c>
+      <c r="I16" s="1">
+        <v>360</v>
+      </c>
+      <c r="J16" s="2">
+        <f>H16*100</f>
+        <v>349.02548789595829</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="2"/>
+        <v>-3.0484755844560299E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>400</v>
       </c>
@@ -4963,8 +5185,19 @@
         <f t="shared" si="1"/>
         <v>5.0671283463087722</v>
       </c>
+      <c r="I17" s="1">
+        <v>400</v>
+      </c>
+      <c r="J17" s="2">
+        <f>H17*100</f>
+        <v>506.71283463087724</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.2667820865771931</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>440</v>
       </c>
@@ -4988,8 +5221,19 @@
         <f t="shared" si="1"/>
         <v>3.810240429946278</v>
       </c>
+      <c r="I18" s="1">
+        <v>440</v>
+      </c>
+      <c r="J18" s="2">
+        <f>H18*100</f>
+        <v>381.02404299462779</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.13403626592130047</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>480</v>
       </c>
@@ -5013,8 +5257,19 @@
         <f t="shared" si="1"/>
         <v>2.5118864315095815</v>
       </c>
+      <c r="I19" s="1">
+        <v>480</v>
+      </c>
+      <c r="J19" s="2">
+        <f>H19*100</f>
+        <v>251.18864315095814</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.47669032676883721</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>520</v>
       </c>
@@ -5038,8 +5293,19 @@
         <f t="shared" si="1"/>
         <v>5.1794746792312116</v>
       </c>
+      <c r="I20" s="1">
+        <v>520</v>
+      </c>
+      <c r="J20" s="2">
+        <f>H20*100</f>
+        <v>517.94746792312117</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="2"/>
+        <v>-3.9471770709208331E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>560</v>
       </c>
@@ -5062,6 +5328,23 @@
       <c r="H21">
         <f t="shared" si="1"/>
         <v>6.8880333009565717</v>
+      </c>
+      <c r="I21" s="1">
+        <v>560</v>
+      </c>
+      <c r="J21" s="2">
+        <f>H21*100</f>
+        <v>688.8033300956572</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.23000594659938786</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="4" cm="1">
+        <f t="array" ref="K23">SUM(ABS(K3:K21))/COUNT(K3:K21)</f>
+        <v>0.21392413373517086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report finished, Excel files updated with graph tweaking
</commit_message>
<xml_diff>
--- a/Measurements/Test 1 - No obstacles/Statistics2.xlsx
+++ b/Measurements/Test 1 - No obstacles/Statistics2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\code\SerialReading\Measurements\Test 1 - No obstacles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\Proyects\Work\Vamia-SerialPortReading\Measurements\Test 1 - No obstacles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5ABA5A-31AD-4E48-B0BE-D38AF5100F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24C05A3-5403-4C5E-85D0-B1B10C530AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1679,61 +1679,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>45.121629908943603</c:v>
+                  <c:v>45.421629908943608</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.44325981788721</c:v>
+                  <c:v>51.743259817887214</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.141176258056511</c:v>
+                  <c:v>55.441176258056515</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.764889726830816</c:v>
+                  <c:v>58.06488972683082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59.8</c:v>
+                  <c:v>60.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.462806167000117</c:v>
+                  <c:v>61.762806167000122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.868688749242992</c:v>
+                  <c:v>63.168688749242996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.086519635774422</c:v>
+                  <c:v>64.38651963577442</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65.160722607169419</c:v>
+                  <c:v>65.46072260716943</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.121629908943603</c:v>
+                  <c:v>66.421629908943601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67.784436075943717</c:v>
+                  <c:v>68.084436075943728</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69.190318658186598</c:v>
+                  <c:v>69.490318658186609</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70.408149544718015</c:v>
+                  <c:v>70.708149544718026</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.482352516113025</c:v>
+                  <c:v>71.782352516113036</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>72.44325981788721</c:v>
+                  <c:v>72.743259817887207</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>73.312506206209932</c:v>
+                  <c:v>73.612506206209943</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74.106065984887323</c:v>
+                  <c:v>74.406065984887334</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>74.836070216330782</c:v>
+                  <c:v>75.136070216330779</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75.511948567130204</c:v>
+                  <c:v>75.811948567130202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4293,16 +4293,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>245745</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>112395</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>43815</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4618,16 +4618,16 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="I3" sqref="I3:K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4635,14 +4635,13 @@
         <v>1</v>
       </c>
       <c r="F1">
-        <f>B7</f>
-        <v>59.8</v>
+        <v>60.1</v>
       </c>
       <c r="G1">
         <v>2.1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4657,7 +4656,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -4675,25 +4674,25 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F21" si="0">10*$G$1*LOG(A3/100,10)+$F$1</f>
-        <v>45.121629908943603</v>
+        <v>45.421629908943608</v>
       </c>
       <c r="H3">
         <f>POWER(10, (B3-$F$1)/(10*$G$1))</f>
-        <v>0.26245062966121019</v>
+        <v>0.25395800383208283</v>
       </c>
       <c r="I3" s="1">
         <v>20</v>
       </c>
       <c r="J3" s="2">
-        <f>H3*100</f>
-        <v>26.245062966121019</v>
+        <f t="shared" ref="J3:J21" si="1">H3*100</f>
+        <v>25.395800383208282</v>
       </c>
       <c r="K3" s="3">
         <f>(J3-I3)/I3</f>
-        <v>0.31225314830605094</v>
+        <v>0.26979001916041412</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>40</v>
       </c>
@@ -4711,25 +4710,25 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>51.44325981788721</v>
+        <v>51.743259817887214</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H21" si="1">POWER(10, (B4-$F$1)/(10*$G$1))</f>
-        <v>0.44424141892319974</v>
+        <f t="shared" ref="H4:H21" si="2">POWER(10, (B4-$F$1)/(10*$G$1))</f>
+        <v>0.42986623470822749</v>
       </c>
       <c r="I4" s="1">
         <v>40</v>
       </c>
       <c r="J4" s="2">
-        <f>H4*100</f>
-        <v>44.424141892319973</v>
+        <f t="shared" si="1"/>
+        <v>42.986623470822749</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K21" si="2">(J4-I4)/I4</f>
-        <v>0.11060354730799933</v>
+        <f t="shared" ref="K4:K21" si="3">(J4-I4)/I4</f>
+        <v>7.466558677056874E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -4747,25 +4746,25 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>55.141176258056511</v>
+        <v>55.441176258056515</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>0.78566624593889489</v>
+        <f t="shared" si="2"/>
+        <v>0.76024291408426248</v>
       </c>
       <c r="I5" s="1">
         <v>60</v>
       </c>
       <c r="J5" s="2">
-        <f>H5*100</f>
-        <v>78.566624593889486</v>
+        <f t="shared" si="1"/>
+        <v>76.024291408426251</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="2"/>
-        <v>0.30944374323149143</v>
+        <f t="shared" si="3"/>
+        <v>0.26707152347377083</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>80</v>
       </c>
@@ -4783,25 +4782,25 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>57.764889726830816</v>
+        <v>58.06488972683082</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1.3298710250629042</v>
+        <f t="shared" si="2"/>
+        <v>1.2868377999895388</v>
       </c>
       <c r="I6" s="1">
         <v>80</v>
       </c>
       <c r="J6" s="2">
-        <f>H6*100</f>
-        <v>132.98710250629043</v>
+        <f t="shared" si="1"/>
+        <v>128.6837799989539</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.66233878132863033</v>
+        <f t="shared" si="3"/>
+        <v>0.60854724998692367</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>100</v>
       </c>
@@ -4819,25 +4818,25 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>59.8</v>
+        <v>60.1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.96764105370945297</v>
       </c>
       <c r="I7" s="1">
         <v>100</v>
       </c>
       <c r="J7" s="2">
-        <f>H7*100</f>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>96.764105370945302</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>-3.2358946290546982E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>120</v>
       </c>
@@ -4855,25 +4854,25 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>61.462806167000117</v>
+        <v>61.762806167000122</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1.0221715980421691</v>
+        <f t="shared" si="2"/>
+        <v>0.98909520220140001</v>
       </c>
       <c r="I8" s="1">
         <v>120</v>
       </c>
       <c r="J8" s="2">
-        <f>H8*100</f>
-        <v>102.21715980421691</v>
+        <f t="shared" si="1"/>
+        <v>98.909520220139996</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="2"/>
-        <v>-0.14819033496485912</v>
+        <f t="shared" si="3"/>
+        <v>-0.17575399816550002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>140</v>
       </c>
@@ -4891,25 +4890,25 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>62.868688749242992</v>
+        <v>63.168688749242996</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>1.9735043828689784</v>
+        <f t="shared" si="2"/>
+        <v>1.9096438605395625</v>
       </c>
       <c r="I9" s="1">
         <v>140</v>
       </c>
       <c r="J9" s="2">
-        <f>H9*100</f>
-        <v>197.35043828689786</v>
+        <f t="shared" si="1"/>
+        <v>190.96438605395625</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.4096459877635561</v>
+        <f t="shared" si="3"/>
+        <v>0.36403132895683032</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>160</v>
       </c>
@@ -4927,25 +4926,25 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>64.086519635774422</v>
+        <v>64.38651963577442</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1.7685569433018593</v>
+        <f t="shared" si="2"/>
+        <v>1.7113283041617806</v>
       </c>
       <c r="I10" s="1">
         <v>160</v>
       </c>
       <c r="J10" s="2">
-        <f>H10*100</f>
-        <v>176.85569433018594</v>
+        <f t="shared" si="1"/>
+        <v>171.13283041617805</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="2"/>
-        <v>0.10534808956366212</v>
+        <f t="shared" si="3"/>
+        <v>6.9580190101112827E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>180</v>
       </c>
@@ -4963,25 +4962,25 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>65.160722607169419</v>
+        <v>65.46072260716943</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>2.0619860095022222</v>
+        <f t="shared" si="2"/>
+        <v>1.9952623149688808</v>
       </c>
       <c r="I11" s="1">
         <v>180</v>
       </c>
       <c r="J11" s="2">
-        <f>H11*100</f>
-        <v>206.19860095022221</v>
+        <f t="shared" si="1"/>
+        <v>199.52623149688807</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="2"/>
-        <v>0.14554778305679009</v>
+        <f t="shared" si="3"/>
+        <v>0.1084790638716004</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>200</v>
       </c>
@@ -4999,25 +4998,25 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>66.121629908943603</v>
+        <v>66.421629908943601</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>1.8888195803730405</v>
+        <f t="shared" si="2"/>
+        <v>1.827699369019216</v>
       </c>
       <c r="I12" s="1">
         <v>200</v>
       </c>
       <c r="J12" s="2">
-        <f>H12*100</f>
-        <v>188.88195803730406</v>
+        <f t="shared" si="1"/>
+        <v>182.7699369019216</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="2"/>
-        <v>-5.5590209813479702E-2</v>
+        <f t="shared" si="3"/>
+        <v>-8.6150315490392024E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>240</v>
       </c>
@@ -5035,25 +5034,25 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>67.784436075943717</v>
+        <v>68.084436075943728</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>1.6200328072641321</v>
+        <f t="shared" si="2"/>
+        <v>1.567610252664948</v>
       </c>
       <c r="I13" s="1">
         <v>240</v>
       </c>
       <c r="J13" s="2">
-        <f>H13*100</f>
-        <v>162.00328072641321</v>
+        <f t="shared" si="1"/>
+        <v>156.76102526649481</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="2"/>
-        <v>-0.32498633030661161</v>
+        <f t="shared" si="3"/>
+        <v>-0.34682906138960495</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>280</v>
       </c>
@@ -5071,25 +5070,25 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>69.190318658186598</v>
+        <v>69.490318658186609</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>3.5676394072005944</v>
+        <f t="shared" si="2"/>
+        <v>3.452194355238952</v>
       </c>
       <c r="I14" s="1">
         <v>280</v>
       </c>
       <c r="J14" s="2">
-        <f>H14*100</f>
-        <v>356.76394072005945</v>
+        <f t="shared" si="1"/>
+        <v>345.21943552389519</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="2"/>
-        <v>0.27415693114306949</v>
+        <f t="shared" si="3"/>
+        <v>0.23292655544248281</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>320</v>
       </c>
@@ -5107,25 +5106,25 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>70.408149544718015</v>
+        <v>70.708149544718026</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
-        <v>2.9935772947204904</v>
+        <f t="shared" si="2"/>
+        <v>2.8967082878240289</v>
       </c>
       <c r="I15" s="1">
         <v>320</v>
       </c>
       <c r="J15" s="2">
-        <f>H15*100</f>
-        <v>299.35772947204902</v>
+        <f t="shared" si="1"/>
+        <v>289.67082878240291</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="2"/>
-        <v>-6.4507095399846823E-2</v>
+        <f t="shared" si="3"/>
+        <v>-9.4778660054990915E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>360</v>
       </c>
@@ -5143,25 +5142,25 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>71.482352516113025</v>
+        <v>71.782352516113036</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
-        <v>3.4902548789595831</v>
+        <f t="shared" si="2"/>
+        <v>3.3773139087910109</v>
       </c>
       <c r="I16" s="1">
         <v>360</v>
       </c>
       <c r="J16" s="2">
-        <f>H16*100</f>
-        <v>349.02548789595829</v>
+        <f t="shared" si="1"/>
+        <v>337.73139087910107</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="2"/>
-        <v>-3.0484755844560299E-2</v>
+        <f t="shared" si="3"/>
+        <v>-6.185724755805258E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>400</v>
       </c>
@@ -5179,25 +5178,25 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>72.44325981788721</v>
+        <v>72.743259817887207</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
-        <v>5.0671283463087722</v>
+        <f t="shared" si="2"/>
+        <v>4.903161412303259</v>
       </c>
       <c r="I17" s="1">
         <v>400</v>
       </c>
       <c r="J17" s="2">
-        <f>H17*100</f>
-        <v>506.71283463087724</v>
+        <f t="shared" si="1"/>
+        <v>490.31614123032591</v>
       </c>
       <c r="K17" s="3">
-        <f t="shared" si="2"/>
-        <v>0.2667820865771931</v>
+        <f t="shared" si="3"/>
+        <v>0.22579035307581477</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>440</v>
       </c>
@@ -5215,25 +5214,25 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>73.312506206209932</v>
+        <v>73.612506206209943</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
-        <v>3.810240429946278</v>
+        <f t="shared" si="2"/>
+        <v>3.6869450645195756</v>
       </c>
       <c r="I18" s="1">
         <v>440</v>
       </c>
       <c r="J18" s="2">
-        <f>H18*100</f>
-        <v>381.02404299462779</v>
+        <f t="shared" si="1"/>
+        <v>368.69450645195758</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="2"/>
-        <v>-0.13403626592130047</v>
+        <f t="shared" si="3"/>
+        <v>-0.16205793988191458</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>480</v>
       </c>
@@ -5251,25 +5250,25 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>74.106065984887323</v>
+        <v>74.406065984887334</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
-        <v>2.5118864315095815</v>
+        <f t="shared" si="2"/>
+        <v>2.4306044333844099</v>
       </c>
       <c r="I19" s="1">
         <v>480</v>
       </c>
       <c r="J19" s="2">
-        <f>H19*100</f>
-        <v>251.18864315095814</v>
+        <f t="shared" si="1"/>
+        <v>243.06044333844099</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="2"/>
-        <v>-0.47669032676883721</v>
+        <f t="shared" si="3"/>
+        <v>-0.49362407637824796</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>520</v>
       </c>
@@ -5287,25 +5286,25 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>74.836070216330782</v>
+        <v>75.136070216330779</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
-        <v>5.1794746792312116</v>
+        <f t="shared" si="2"/>
+        <v>5.011872336272722</v>
       </c>
       <c r="I20" s="1">
         <v>520</v>
       </c>
       <c r="J20" s="2">
-        <f>H20*100</f>
-        <v>517.94746792312117</v>
+        <f t="shared" si="1"/>
+        <v>501.18723362727218</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="2"/>
-        <v>-3.9471770709208331E-3</v>
+        <f t="shared" si="3"/>
+        <v>-3.6178396870630423E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>560</v>
       </c>
@@ -5323,28 +5322,28 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>75.511948567130204</v>
+        <v>75.811948567130202</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
-        <v>6.8880333009565717</v>
+        <f t="shared" si="2"/>
+        <v>6.6651438013234205</v>
       </c>
       <c r="I21" s="1">
         <v>560</v>
       </c>
       <c r="J21" s="2">
-        <f>H21*100</f>
-        <v>688.8033300956572</v>
+        <f t="shared" si="1"/>
+        <v>666.51438013234201</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="2"/>
-        <v>0.23000594659938786</v>
+        <f t="shared" si="3"/>
+        <v>0.19020425023632503</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K23" s="4" cm="1">
         <f t="array" ref="K23">SUM(ABS(K3:K21))/COUNT(K3:K21)</f>
-        <v>0.21392413373517086</v>
+        <v>0.2052986717450381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added strategy to handle data from Serial Port
</commit_message>
<xml_diff>
--- a/Measurements/Test 1 - No obstacles/Statistics2.xlsx
+++ b/Measurements/Test 1 - No obstacles/Statistics2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\Proyects\Work\Vamia-SerialPortReading\Measurements\Test 1 - No obstacles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24C05A3-5403-4C5E-85D0-B1B10C530AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F700E77-CA7E-4B5E-8403-34B9057CD4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4615,10 +4615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:K21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5346,6 +5346,12 @@
         <v>0.2052986717450381</v>
       </c>
     </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f>SUM(C2:C21)/COUNT(C2:C21)</f>
+        <v>1.8028709576742077</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>